<commit_message>
Changes from our call 30th 12
</commit_message>
<xml_diff>
--- a/scenarios/bladder/processes/Bladder.xlsx
+++ b/scenarios/bladder/processes/Bladder.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamim\Documents\GitHub\dein-apotheker-scenarios\scenarios\bladder\processes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0028A4E2-6A01-44F8-8082-9AC54F35116B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="content" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="content" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,266 +27,247 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Query</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Popup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bladder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wie genau kann ich dir weiterhelfen?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[question]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich habe eine Blasenentzündung.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(diagnosis)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meds</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Hint</t>
+  </si>
+  <si>
+    <t>Popup</t>
+  </si>
+  <si>
+    <t>bladder</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Wie genau kann ich dir weiterhelfen?</t>
+  </si>
+  <si>
+    <t>[question]</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Ich habe eine Blasenentzündung.</t>
+  </si>
+  <si>
+    <t>GO(diagnosis)</t>
+  </si>
+  <si>
+    <t>meds</t>
   </si>
   <si>
     <t xml:space="preserve">Habe ich eine Blasenentzündung? </t>
   </si>
   <si>
-    <t xml:space="preserve">JUMP(Bladder_symptomcheck)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich bekomme immer wieder eine Blasenentzündung. Habe aber im Moment gerade keine.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(frequency)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rezidiv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diagnosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hat ein Arzt deine Blasenentzündung diagnostiziert?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUMP(Antibiotic_combi)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(repeat)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repeat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First time?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hattest du schon einmal eine Blasenentzündung?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(check)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptom-Check?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wollen wir einmal checken, wie wahrscheinlich es eine Blasenentzündung ist?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(meds)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Right Meds?</t>
+    <t>JUMP(Bladder_symptomcheck)</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Ich bekomme immer wieder eine Blasenentzündung. Habe aber im Moment gerade keine.</t>
+  </si>
+  <si>
+    <t>GO(frequency)</t>
+  </si>
+  <si>
+    <t>rezidiv</t>
+  </si>
+  <si>
+    <t>diagnosis</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>Hat ein Arzt deine Blasenentzündung diagnostiziert?</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>JUMP(Antibiotic_combi)</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>GO(repeat)</t>
+  </si>
+  <si>
+    <t>repeat</t>
+  </si>
+  <si>
+    <t>First time?</t>
+  </si>
+  <si>
+    <t>Hattest du schon einmal eine Blasenentzündung?</t>
+  </si>
+  <si>
+    <t>GO(check)</t>
+  </si>
+  <si>
+    <t>Symptom-Check?</t>
+  </si>
+  <si>
+    <t>Wollen wir einmal checken, wie wahrscheinlich es eine Blasenentzündung ist?</t>
+  </si>
+  <si>
+    <t>GO(meds)</t>
+  </si>
+  <si>
+    <t>Right Meds?</t>
   </si>
   <si>
     <t xml:space="preserve">Wollen wir das richtige Medikament für dich finden? </t>
   </si>
   <si>
-    <t xml:space="preserve">Go(WhatThen)</t>
+    <t>Go(WhatThen)</t>
   </si>
   <si>
     <t xml:space="preserve">frequency </t>
   </si>
   <si>
-    <t xml:space="preserve">How often?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wie oft hattest du dieses Jahr schon eine Blasenentzündung?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[frequency]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In den letzen 12 Monaten noch gar nicht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">first</t>
+    <t>How often?</t>
+  </si>
+  <si>
+    <t>Wie oft hattest du dieses Jahr schon eine Blasenentzündung?</t>
+  </si>
+  <si>
+    <t>[frequency]</t>
+  </si>
+  <si>
+    <t>In den letzen 12 Monaten noch gar nicht</t>
+  </si>
+  <si>
+    <t>first</t>
   </si>
   <si>
     <t xml:space="preserve">Ich hatte in den letzten 12 Monaten schonmal eine </t>
   </si>
   <si>
-    <t xml:space="preserve">GO(rezidiv)</t>
+    <t>GO(rezidiv)</t>
   </si>
   <si>
     <t xml:space="preserve">repeated </t>
   </si>
   <si>
-    <t xml:space="preserve">mindestens 2 mal in den letzten 6 Monaten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mindestens 3 mal in den letzten 12 Monaten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acute or Prophy?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Möchtest du über die akut-Therapie sprechen oder über die Prophylaxe?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Was bedeutet das?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die akut-Therapie ist das, was man machen kann, wenn man gerade eine Blasenentzündung hat und unter den entsprechenden Symptomen leidet. 
+    <t>mindestens 2 mal in den letzten 6 Monaten</t>
+  </si>
+  <si>
+    <t>mindestens 3 mal in den letzten 12 Monaten</t>
+  </si>
+  <si>
+    <t>Acute or Prophy?</t>
+  </si>
+  <si>
+    <t>Möchtest du über die akut-Therapie sprechen oder über die Prophylaxe?</t>
+  </si>
+  <si>
+    <t>Was bedeutet das?</t>
+  </si>
+  <si>
+    <t>Die akut-Therapie ist das, was man machen kann, wenn man gerade eine Blasenentzündung hat und unter den entsprechenden Symptomen leidet. 
 Eine Prophylaxe soll dagegen verhindern, dass es überhaupt erst zur Blasenenetzündung kommt.</t>
   </si>
   <si>
-    <t xml:space="preserve">Akut-Therapie</t>
+    <t>Akut-Therapie</t>
   </si>
   <si>
     <t xml:space="preserve">Prophylaxe(Vorbeugung) </t>
   </si>
   <si>
-    <t xml:space="preserve">JUMP(Bladder_rezidiv)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need antibiotics?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wenn deine Symptome nach 5 Tagen nicht besser geworden sind oder sich verschlimmern, dann rate ich dir einen Arzt zu consultieren.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Okay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(antibiotics)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">antibiotics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oft ist bei einer sog. unkomplizierten Blasenentzündung gar keine Antibiotika Therapie notwendig. Dein Körper ist stärker als du denkst.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erzähl mir mehr dazu.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In einer aktuellen Studie wurde der Effekt einer Antibiotika-Therapie mit dem Effekt einer rein symptomatischen Therapie (Ibuprofen, ein herkömmliches Schmerzmittel)  verglichen: Nach einer Woche sind 70% der Patientinnen, die ohne Antibiotikum behandelt wurden, beschwerdefrei. In der Gruppe, die mit Antibiotikum behandelt wurden, waren es 80%. 
+    <t>JUMP(Bladder_rezidiv)</t>
+  </si>
+  <si>
+    <t>Need antibiotics?</t>
+  </si>
+  <si>
+    <t>Wenn deine Symptome nach 5 Tagen nicht besser geworden sind oder sich verschlimmern, dann rate ich dir einen Arzt zu consultieren.</t>
+  </si>
+  <si>
+    <t>Okay</t>
+  </si>
+  <si>
+    <t>GO(antibiotics)</t>
+  </si>
+  <si>
+    <t>antibiotics</t>
+  </si>
+  <si>
+    <t>Oft ist bei einer sog. unkomplizierten Blasenentzündung gar keine Antibiotika Therapie notwendig. Dein Körper ist stärker als du denkst.</t>
+  </si>
+  <si>
+    <t>Erzähl mir mehr dazu.</t>
+  </si>
+  <si>
+    <t>In einer aktuellen Studie wurde der Effekt einer Antibiotika-Therapie mit dem Effekt einer rein symptomatischen Therapie (Ibuprofen, ein herkömmliches Schmerzmittel)  verglichen: Nach einer Woche sind 70% der Patientinnen, die ohne Antibiotikum behandelt wurden, beschwerdefrei. In der Gruppe, die mit Antibiotikum behandelt wurden, waren es 80%. 
 Daher empfiehlt die aktuelle Leitlinie der Deutschen Gesellschaft für Urologie Patientinnen die Wahl zu überlassen: Ohne Antibiotika-Therapie können unter Inkaufnahme einer höheren Symptomlast eventuelle Nebenwirkungen des Antibiotikums umgangen werden. - Deutsche Gesellschaft für Urologie (https://www.awmf.org/uploads/tx_szleitlinien/043-044l_S3_Harnwegsinfektionen_2017-05.pdf)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ich möchte es ohne Antibiotika versuchen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(meds2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich möchte ein Antibiotikum einnehmen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(antibiotics2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">antibiotics2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antibiotika sind verschreibungspflichtig. Dabei kann ich dir im Moment leider nicht weiterhelfen. Ich habe im Ratgeber Informationen zu dem Thema bereitgestellt, wo ich dir z.B. in Videos mehr zu der Thematik erkläre.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(clip_Antibiotics); JUMP(Antibiotic_combi)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meds2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich werde dir jetzt ein paar wenige Fragen stellen unter welchen Symptomen du genau leidest.</t>
+    <t>Ich möchte es ohne Antibiotika versuchen.</t>
+  </si>
+  <si>
+    <t>GO(meds2)</t>
+  </si>
+  <si>
+    <t>Ich möchte ein Antibiotikum einnehmen.</t>
+  </si>
+  <si>
+    <t>GO(antibiotics2)</t>
+  </si>
+  <si>
+    <t>antibiotics2</t>
+  </si>
+  <si>
+    <t>Antibiotika sind verschreibungspflichtig. Dabei kann ich dir im Moment leider nicht weiterhelfen. Ich habe im Ratgeber Informationen zu dem Thema bereitgestellt, wo ich dir z.B. in Videos mehr zu der Thematik erkläre.</t>
+  </si>
+  <si>
+    <t>GO(clip_Antibiotics); JUMP(Antibiotic_combi)</t>
+  </si>
+  <si>
+    <t>meds2</t>
+  </si>
+  <si>
+    <t>Ich werde dir jetzt ein paar wenige Fragen stellen unter welchen Symptomen du genau leidest.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -291,7 +277,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -299,7 +285,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -341,14 +327,14 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFF4B183"/>
       </left>
@@ -361,7 +347,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FFF4B183"/>
       </left>
@@ -373,114 +359,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="13" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="13"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="MetaData_Columns" xfId="20"/>
+  <cellStyles count="2">
+    <cellStyle name="MetaData_Columns" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -539,34 +475,342 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF3652A0"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="46.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="40.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.15"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="13.53515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.53515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.921875" customWidth="1"/>
+    <col min="8" max="8" width="16.765625" customWidth="1"/>
+    <col min="9" max="9" width="51.3828125" style="2" customWidth="1"/>
+    <col min="1024" max="1024" width="9.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,11 +835,11 @@
       <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -610,11 +854,11 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
@@ -627,11 +871,11 @@
         <v>16</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="8" t="s">
@@ -644,11 +888,11 @@
         <v>19</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="0" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
@@ -661,11 +905,11 @@
         <v>22</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="0" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>24</v>
       </c>
@@ -681,7 +925,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="s">
@@ -695,7 +939,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="8" t="s">
@@ -710,7 +954,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
@@ -727,7 +971,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8" t="s">
@@ -742,7 +986,7 @@
       <c r="F10" s="10"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8" t="s">
@@ -757,7 +1001,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -774,7 +1018,7 @@
       <c r="F12" s="10"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
@@ -789,7 +1033,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
@@ -804,7 +1048,7 @@
       <c r="F14" s="10"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:9" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -821,7 +1065,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8" t="s">
@@ -836,7 +1080,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="s">
@@ -851,7 +1095,7 @@
       <c r="F17" s="10"/>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
@@ -870,7 +1114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="s">
@@ -887,7 +1131,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8" t="s">
@@ -896,7 +1140,7 @@
       <c r="D20" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" t="s">
         <v>48</v>
       </c>
       <c r="F20" s="10"/>
@@ -904,7 +1148,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8" t="s">
@@ -913,7 +1157,7 @@
       <c r="D21" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" t="s">
         <v>48</v>
       </c>
       <c r="F21" s="10"/>
@@ -921,7 +1165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="13"/>
       <c r="C22" s="8" t="s">
         <v>14</v>
@@ -936,8 +1180,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="13" t="s">
@@ -957,7 +1201,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="13"/>
       <c r="C24" s="8" t="s">
         <v>14</v>
@@ -969,7 +1213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="13"/>
       <c r="C25" s="8" t="s">
         <v>14</v>
@@ -981,8 +1225,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:9" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -996,7 +1240,7 @@
       </c>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" customFormat="false" ht="15.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="13"/>
       <c r="C27" s="14" t="s">
         <v>14</v>
@@ -1004,13 +1248,13 @@
       <c r="D27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" t="s">
         <v>62</v>
       </c>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:9" ht="218.6" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="13"/>
@@ -1028,7 +1272,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
         <v>14</v>
@@ -1036,12 +1280,12 @@
       <c r="D29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" t="s">
         <v>68</v>
       </c>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
         <v>14</v>
@@ -1049,13 +1293,13 @@
       <c r="D30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" t="s">
         <v>70</v>
       </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
         <v>71</v>
       </c>
       <c r="B31" s="13"/>
@@ -1067,7 +1311,7 @@
       </c>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
         <v>14</v>
@@ -1080,8 +1324,8 @@
       </c>
       <c r="F32" s="15"/>
     </row>
-    <row r="33" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
         <v>74</v>
       </c>
       <c r="B33" s="13"/>
@@ -1093,7 +1337,7 @@
       </c>
       <c r="F33" s="15"/>
     </row>
-    <row r="34" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B34" s="13"/>
       <c r="C34" s="14" t="s">
         <v>14</v>
@@ -1101,22 +1345,13 @@
       <c r="D34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" t="s">
         <v>19</v>
       </c>
       <c r="F34" s="15"/>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>